<commit_message>
I will Modify The Database soon.. check the Flow Diagram
</commit_message>
<xml_diff>
--- a/DataBase/Project Database.xlsx
+++ b/DataBase/Project Database.xlsx
@@ -1,43 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9af0ff2da4243c3f/Desktop/Share Steer/DataBase/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projectCdac\Cdac-Project-Group10\Share-Steer-Ride-Sharing-App\DataBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{254F568F-AB34-4245-A418-02B61F4B8D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F0F778-FA24-4559-A194-9A928C926286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3A6159D2-3324-4254-BB3B-A738DEB51357}"/>
+    <workbookView xWindow="28680" yWindow="945" windowWidth="20730" windowHeight="11760" xr2:uid="{3A6159D2-3324-4254-BB3B-A738DEB51357}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
-  <si>
-    <t>age(Autogenerated)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Email</t>
   </si>
@@ -60,9 +49,6 @@
     <t>user_name(uniqueId)</t>
   </si>
   <si>
-    <t>Passenger</t>
-  </si>
-  <si>
     <t>address</t>
   </si>
   <si>
@@ -72,15 +58,9 @@
     <t>city</t>
   </si>
   <si>
-    <t>Driver</t>
-  </si>
-  <si>
     <t>rating</t>
   </si>
   <si>
-    <t>Driver_id(Primary Key)</t>
-  </si>
-  <si>
     <t>Passenger_id(Primary Key)</t>
   </si>
   <si>
@@ -157,6 +137,12 @@
   </si>
   <si>
     <t>status</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Vehicle Details</t>
   </si>
 </sst>
 </file>
@@ -180,7 +166,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -212,11 +198,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -236,7 +235,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -553,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{993FF97A-B2EE-41F0-969E-88BF8C41B4DF}">
-  <dimension ref="A2:R60"/>
+  <dimension ref="A2:S60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -571,70 +588,67 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
+      <c r="A2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-    </row>
-    <row r="4" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+    </row>
+    <row r="4" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>9</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
@@ -644,13 +658,12 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="G5" s="13"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
+      <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
@@ -659,13 +672,12 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="G6" s="13"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
+      <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
@@ -674,13 +686,12 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="G7" s="13"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
+      <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
@@ -703,172 +714,146 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
+      <c r="H9" s="1"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+    </row>
+    <row r="12" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="7"/>
-      <c r="R11" s="7"/>
-    </row>
-    <row r="12" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="L12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="M12" s="4" t="s">
+      <c r="B12" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="N12" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="O12" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="P12" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q12" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="R12" s="4" t="s">
+      <c r="F12" s="11"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="11"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="11"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="4"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="4"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="4"/>
-      <c r="R15" s="4"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
-        <v>17</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -886,7 +871,7 @@
       <c r="O18" s="6"/>
       <c r="P18" s="6"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -904,49 +889,50 @@
       <c r="O19" s="6"/>
       <c r="P19" s="6"/>
     </row>
-    <row r="20" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K20" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="L20" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="1"/>
-      <c r="R20" s="1"/>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+      <c r="S20" s="5"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>1</v>
       </c>
@@ -954,11 +940,11 @@
         <v>1</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1">
@@ -966,7 +952,7 @@
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J21" s="1">
         <v>9</v>
@@ -975,12 +961,15 @@
         <v>4</v>
       </c>
       <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5"/>
+      <c r="S21" s="5"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -993,12 +982,15 @@
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="5"/>
+      <c r="S22" s="5"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1011,12 +1003,15 @@
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
-      <c r="P23" s="1"/>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="5"/>
+      <c r="R23" s="5"/>
+      <c r="S23" s="5"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1029,12 +1024,15 @@
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
-      <c r="P24" s="1"/>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="5"/>
+      <c r="R24" s="5"/>
+      <c r="S24" s="5"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1047,12 +1045,15 @@
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
-      <c r="P25" s="1"/>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="5"/>
+      <c r="R25" s="5"/>
+      <c r="S25" s="5"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1065,12 +1066,15 @@
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
-      <c r="P26" s="1"/>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="5"/>
+      <c r="R26" s="5"/>
+      <c r="S26" s="5"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1083,32 +1087,44 @@
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
-      <c r="N27" s="1"/>
-      <c r="O27" s="1"/>
-      <c r="P27" s="1"/>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="5"/>
+      <c r="R27" s="5"/>
+      <c r="S27" s="5"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
+      <c r="P28" s="5"/>
+      <c r="Q28" s="5"/>
+      <c r="R28" s="5"/>
+      <c r="S28" s="5"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -1152,10 +1168,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updating Sql and Flow diagram
</commit_message>
<xml_diff>
--- a/DataBase/Project Database.xlsx
+++ b/DataBase/Project Database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projectCdac\Cdac-Project-Group10\Share-Steer-Ride-Sharing-App\DataBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F0F778-FA24-4559-A194-9A928C926286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{116D51A0-FF44-45CB-B175-A3C79ECD4B6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="945" windowWidth="20730" windowHeight="11760" xr2:uid="{3A6159D2-3324-4254-BB3B-A738DEB51357}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{3A6159D2-3324-4254-BB3B-A738DEB51357}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
   <si>
     <t>Email</t>
   </si>
@@ -61,18 +61,12 @@
     <t>rating</t>
   </si>
   <si>
-    <t>Passenger_id(Primary Key)</t>
-  </si>
-  <si>
     <t>driving licence(Unique)</t>
   </si>
   <si>
     <t>Rides</t>
   </si>
   <si>
-    <t>driver_id</t>
-  </si>
-  <si>
     <t>source</t>
   </si>
   <si>
@@ -143,6 +137,9 @@
   </si>
   <si>
     <t>Vehicle Details</t>
+  </si>
+  <si>
+    <t>user id(Primary Key)</t>
   </si>
 </sst>
 </file>
@@ -232,18 +229,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -254,6 +239,18 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -572,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{993FF97A-B2EE-41F0-969E-88BF8C41B4DF}">
   <dimension ref="A2:S60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F42" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -588,34 +585,34 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
+      <c r="A2" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
     </row>
     <row r="4" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>6</v>
@@ -632,8 +629,8 @@
       <c r="F4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="13" t="s">
-        <v>24</v>
+      <c r="G4" s="9" t="s">
+        <v>22</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>1</v>
@@ -658,7 +655,7 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="13"/>
+      <c r="G5" s="9"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="4"/>
@@ -672,7 +669,7 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="13"/>
+      <c r="G6" s="9"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="4"/>
@@ -686,7 +683,7 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="13"/>
+      <c r="G7" s="9"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="4"/>
@@ -714,215 +711,217 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="1"/>
+      <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="7"/>
+      <c r="A10" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="9"/>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="9"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
     </row>
     <row r="12" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A18" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="11"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="11"/>
-      <c r="O12" s="11"/>
-      <c r="P12" s="11"/>
-      <c r="Q12" s="11"/>
-      <c r="R12" s="11"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="11"/>
-      <c r="O13" s="11"/>
-      <c r="P13" s="11"/>
-      <c r="Q13" s="11"/>
-      <c r="R13" s="11"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="11"/>
-      <c r="O14" s="11"/>
-      <c r="P14" s="11"/>
-      <c r="Q14" s="11"/>
-      <c r="R14" s="11"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="11"/>
-      <c r="O15" s="11"/>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="11"/>
-      <c r="R15" s="11"/>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="6"/>
-      <c r="P18" s="6"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="13"/>
+      <c r="O18" s="13"/>
+      <c r="P18" s="13"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="6"/>
+      <c r="A19" s="13"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="13"/>
     </row>
     <row r="20" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H20" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="I20" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
@@ -940,11 +939,11 @@
         <v>1</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1">
@@ -952,7 +951,7 @@
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J21" s="1">
         <v>9</v>
@@ -1106,16 +1105,16 @@
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
@@ -1168,10 +1167,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>